<commit_message>
Adiciona arquivos com as métricas dos resultados do RFR nos atributos de qualidade
</commit_message>
<xml_diff>
--- a/Random Forest Regressor/random_forest_results.xlsx
+++ b/Random Forest Regressor/random_forest_results.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,7 +466,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9794807982425596</v>
+        <v>0.9715091710380933</v>
       </c>
     </row>
     <row r="3">
@@ -476,7 +476,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.4611314285714287</v>
+        <v>0.5329992917598274</v>
       </c>
     </row>
     <row r="4">
@@ -486,7 +486,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5823428347141033</v>
+        <v>0.6756218502717789</v>
       </c>
     </row>
     <row r="5">
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>20.88482265392079</v>
+        <v>24.13974627050411</v>
       </c>
     </row>
     <row r="6">
@@ -506,136 +506,226 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>21.92229538241154</v>
+        <v>25.43378382210334</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Training Total Number of Instances</t>
+          <t>Training Slope</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>175</v>
+        <v>1.104845382685307</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CV Correlation coefficient</t>
+          <t>Training Offset</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.8120699275978677</v>
+        <v>-1.479939548353922</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CV Mean absolute error</t>
+          <t>Training R²</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.230902857142857</v>
+        <v>0.9353122640490514</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CV Root mean squared error</t>
+          <t>Training Total Number of Instances</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.550799550462369</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CV Relative absolute error</t>
+          <t>CV Correlation coefficient</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>55.74807155364157</v>
+        <v>0.8255681762290792</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CV Root relative squared error</t>
+          <t>CV Mean absolute error</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>58.37984739837604</v>
+        <v>1.19688141519195</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CV Total Number of Instances</t>
+          <t>CV Root mean squared error</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>175</v>
+        <v>1.499466911243777</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Validation Correlation coefficient</t>
+          <t>CV Relative absolute error</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.8218100915854232</v>
+        <v>54.20722714887707</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Validation Mean absolute error</t>
+          <t>CV Root relative squared error</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9880533333333339</v>
+        <v>56.44743025056103</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Validation Root mean squared error</t>
+          <t>CV Slope</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1.208252865366628</v>
+        <v>1.016308561165662</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Validation Relative absolute error</t>
+          <t>CV Offset</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>57.32763955935143</v>
+        <v>-0.2398723426715481</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Validation Root relative squared error</t>
+          <t>CV R²</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>57.41733658725042</v>
+        <v>0.6813687618108046</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>CV Total Number of Instances</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Validation Correlation coefficient</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.825542682816069</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Validation Mean absolute error</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.9844046951659461</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Validation Root mean squared error</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1.192576089918173</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Validation Relative absolute error</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>57.11594267347905</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Validation Root relative squared error</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>56.67236116171848</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Validation Slope</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.9410386826744511</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Validation Offset</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.8330992627396174</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Validation R²</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.678824348035574</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>Validation Total Number of Instances</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B28" t="n">
         <v>75</v>
       </c>
     </row>
@@ -650,7 +740,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -677,7 +767,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9736796152575082</v>
+        <v>0.952908143502177</v>
       </c>
     </row>
     <row r="3">
@@ -687,7 +777,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.4493868097087864</v>
+        <v>0.5508005654602991</v>
       </c>
     </row>
     <row r="4">
@@ -697,7 +787,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.776914678286205</v>
+        <v>1.001122909128738</v>
       </c>
     </row>
     <row r="5">
@@ -707,7 +797,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>18.84538608828533</v>
+        <v>23.09825097107709</v>
       </c>
     </row>
     <row r="6">
@@ -717,136 +807,226 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>24.69084521357509</v>
+        <v>31.81632614225842</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Training Total Number of Instances</t>
+          <t>Training Slope</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>175</v>
+        <v>1.112338586816846</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CV Correlation coefficient</t>
+          <t>Training Offset</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.7664937317415584</v>
+        <v>-1.714532149969076</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CV Mean absolute error</t>
+          <t>Training R²</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.233736733170181</v>
+        <v>0.8987721390809443</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CV Root mean squared error</t>
+          <t>Training Total Number of Instances</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2.032893656367519</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CV Relative absolute error</t>
+          <t>CV Correlation coefficient</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>51.73771140047177</v>
+        <v>0.7567937532375055</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CV Root relative squared error</t>
+          <t>CV Mean absolute error</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>64.60666017502939</v>
+        <v>1.227315147050491</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CV Total Number of Instances</t>
+          <t>CV Root mean squared error</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>175</v>
+        <v>2.069985295397034</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Validation Correlation coefficient</t>
+          <t>CV Relative absolute error</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.8511308585388588</v>
+        <v>51.46841718197179</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Validation Mean absolute error</t>
+          <t>CV Root relative squared error</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9452472050176677</v>
+        <v>65.78545617874984</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Validation Root mean squared error</t>
+          <t>CV Slope</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1.330086272736036</v>
+        <v>0.9108495481781673</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Validation Relative absolute error</t>
+          <t>CV Offset</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>47.86978353841291</v>
+        <v>1.348179720794773</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Validation Root relative squared error</t>
+          <t>CV R²</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>55.47398664363355</v>
+        <v>0.5672273755353784</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>CV Total Number of Instances</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Validation Correlation coefficient</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.8568693877414089</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Validation Mean absolute error</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.9655580507156084</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Validation Root mean squared error</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1.297206965332906</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Validation Relative absolute error</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>48.8983777324834</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Validation Root relative squared error</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>54.10268743010118</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Validation Slope</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.8621460697810069</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Validation Offset</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1.929220343964849</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Validation R²</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.7072899212840771</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>Validation Total Number of Instances</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B28" t="n">
         <v>75</v>
       </c>
     </row>
@@ -861,7 +1041,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -888,7 +1068,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9833724791768209</v>
+        <v>0.981268591411302</v>
       </c>
     </row>
     <row r="3">
@@ -898,7 +1078,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.3960914285714288</v>
+        <v>0.4676746580403722</v>
       </c>
     </row>
     <row r="4">
@@ -908,7 +1088,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5175956281555266</v>
+        <v>0.5879474230594502</v>
       </c>
     </row>
     <row r="5">
@@ -918,7 +1098,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17.91100532444254</v>
+        <v>21.14795394709578</v>
       </c>
     </row>
     <row r="6">
@@ -928,136 +1108,226 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>19.47918734996417</v>
+        <v>22.12680591317199</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Training Total Number of Instances</t>
+          <t>Training Slope</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>175</v>
+        <v>1.124742197525316</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CV Correlation coefficient</t>
+          <t>Training Offset</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.8618819158533828</v>
+        <v>-1.74096489241804</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CV Mean absolute error</t>
+          <t>Training R²</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.06304</v>
+        <v>0.9510404460080817</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CV Root mean squared error</t>
+          <t>Training Total Number of Instances</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.354795014542263</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CV Relative absolute error</t>
+          <t>CV Correlation coefficient</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>48.0700003248412</v>
+        <v>0.8703972630685527</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CV Root relative squared error</t>
+          <t>CV Mean absolute error</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>50.98633851122182</v>
+        <v>1.093517653378368</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CV Total Number of Instances</t>
+          <t>CV Root mean squared error</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>175</v>
+        <v>1.351270455867804</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Validation Correlation coefficient</t>
+          <t>CV Relative absolute error</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.8648074691071819</v>
+        <v>49.44818064524169</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Validation Mean absolute error</t>
+          <t>CV Root relative squared error</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.8572799999999994</v>
+        <v>50.85369531446532</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Validation Root mean squared error</t>
+          <t>CV Slope</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1.063041974712193</v>
+        <v>1.171210839511276</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Validation Relative absolute error</t>
+          <t>CV Offset</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>49.93476234855542</v>
+        <v>-2.386583113253321</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Validation Root relative squared error</t>
+          <t>CV R²</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>50.5774836701133</v>
+        <v>0.7413901672863528</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>CV Total Number of Instances</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Validation Correlation coefficient</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.8461533818914526</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Validation Mean absolute error</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.8975765734265734</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Validation Root mean squared error</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1.130215962689932</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Validation Relative absolute error</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>52.28195325178084</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Validation Root relative squared error</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>53.77349225756377</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Validation Slope</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.9972604569367692</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Validation Offset</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.1883568134282889</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Validation R²</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.710841153042573</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>Validation Total Number of Instances</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B28" t="n">
         <v>75</v>
       </c>
     </row>
@@ -1072,7 +1342,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1099,7 +1369,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9712030539954102</v>
+        <v>0.9622552473286912</v>
       </c>
     </row>
     <row r="3">
@@ -1109,7 +1379,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.09602434285714286</v>
+        <v>0.1076562973798027</v>
       </c>
     </row>
     <row r="4">
@@ -1119,7 +1389,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1660573426672674</v>
+        <v>0.1899762872157095</v>
       </c>
     </row>
     <row r="5">
@@ -1129,7 +1399,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>21.21852571516804</v>
+        <v>23.78884193721095</v>
       </c>
     </row>
     <row r="6">
@@ -1139,136 +1409,226 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>28.30754601136683</v>
+        <v>32.38497259469503</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Training Total Number of Instances</t>
+          <t>Training Slope</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>175</v>
+        <v>1.222946928147318</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CV Correlation coefficient</t>
+          <t>Training Offset</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.680219037358554</v>
+        <v>-0.2546790900917506</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CV Mean absolute error</t>
+          <t>Training R²</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2518185142857143</v>
+        <v>0.8951213550040852</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CV Root mean squared error</t>
+          <t>Training Total Number of Instances</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.4302289847763796</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CV Relative absolute error</t>
+          <t>CV Correlation coefficient</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>55.64440705286617</v>
+        <v>0.6988876832201018</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CV Root relative squared error</t>
+          <t>CV Mean absolute error</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>73.3404894138513</v>
+        <v>0.2447320608548198</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CV Total Number of Instances</t>
+          <t>CV Root mean squared error</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>175</v>
+        <v>0.4211029453707894</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Validation Correlation coefficient</t>
+          <t>CV Relative absolute error</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.8030241125968819</v>
+        <v>54.0785114697381</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Validation Mean absolute error</t>
+          <t>CV Root relative squared error</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.2057304</v>
+        <v>71.78478717132582</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Validation Root mean squared error</t>
+          <t>CV Slope</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.2750255925545839</v>
+        <v>1.085131976957128</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Validation Relative absolute error</t>
+          <t>CV Offset</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>58.15968522710369</v>
+        <v>-0.1128508255828744</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Validation Root relative squared error</t>
+          <t>CV R²</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>62.95052916095951</v>
+        <v>0.4846944330767456</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>CV Total Number of Instances</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Validation Correlation coefficient</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.8201927138455699</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Validation Mean absolute error</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.2021528462653087</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Validation Root mean squared error</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.2612065213089956</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Validation Relative absolute error</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>57.14831598321609</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Validation Root relative squared error</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>59.78748589890335</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Validation Slope</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.9913323365763156</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Validation Offset</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>-0.06562658270417687</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Validation R²</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.6425456529888434</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>Validation Total Number of Instances</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B28" t="n">
         <v>75</v>
       </c>
     </row>
@@ -1283,7 +1643,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1310,7 +1670,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9741774225500898</v>
+        <v>0.9728391545290642</v>
       </c>
     </row>
     <row r="3">
@@ -1320,7 +1680,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.053936342857143</v>
+        <v>0.0607944953901259</v>
       </c>
     </row>
     <row r="4">
@@ -1330,7 +1690,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.09159142760885763</v>
+        <v>0.09894849427274606</v>
       </c>
     </row>
     <row r="5">
@@ -1340,7 +1700,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>22.44962155858882</v>
+        <v>25.30415193274365</v>
       </c>
     </row>
     <row r="6">
@@ -1350,136 +1710,226 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>29.64486999709513</v>
+        <v>32.02608940271823</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Training Total Number of Instances</t>
+          <t>Training Slope</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>175</v>
+        <v>1.29447626440131</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CV Correlation coefficient</t>
+          <t>Training Offset</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.6182853186277162</v>
+        <v>-0.9653631737087585</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CV Mean absolute error</t>
+          <t>Training R²</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.141133942857143</v>
+        <v>0.89743295975691</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CV Root mean squared error</t>
+          <t>Training Total Number of Instances</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.2429174570307489</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CV Relative absolute error</t>
+          <t>CV Correlation coefficient</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>58.74338967709146</v>
+        <v>0.6025909056865659</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CV Root relative squared error</t>
+          <t>CV Mean absolute error</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>78.62369461533621</v>
+        <v>0.1519869290437154</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CV Total Number of Instances</t>
+          <t>CV Root mean squared error</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>175</v>
+        <v>0.2472772553358085</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Validation Correlation coefficient</t>
+          <t>CV Relative absolute error</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.7853375605085433</v>
+        <v>63.26066726327239</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Validation Mean absolute error</t>
+          <t>CV Root relative squared error</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.1179050666666669</v>
+        <v>80.0348054293197</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Validation Root mean squared error</t>
+          <t>CV Slope</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.1637733408016499</v>
+        <v>1.10781175206129</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Validation Relative absolute error</t>
+          <t>CV Offset</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>50.3007963594995</v>
+        <v>-0.3590176154429359</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Validation Root relative squared error</t>
+          <t>CV R²</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>62.57310327991832</v>
+        <v>0.3594429919890938</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>CV Total Number of Instances</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Validation Correlation coefficient</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.776485057712856</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Validation Mean absolute error</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.1211224032647908</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Validation Root mean squared error</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.1651951163723708</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Validation Relative absolute error</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>51.67338023241928</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Validation Root relative squared error</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>63.11632300781854</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Validation Slope</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.9750462874834026</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Validation Offset</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.08996829648255744</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Validation R²</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.6016329769972716</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>Validation Total Number of Instances</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B28" t="n">
         <v>75</v>
       </c>
     </row>
@@ -1494,7 +1944,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1521,7 +1971,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9683378678870741</v>
+        <v>0.967419307797571</v>
       </c>
     </row>
     <row r="3">
@@ -1531,7 +1981,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>24.19318502857146</v>
+        <v>26.55852368978382</v>
       </c>
     </row>
     <row r="4">
@@ -1541,7 +1991,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>30.74144886774569</v>
+        <v>33.97305224416854</v>
       </c>
     </row>
     <row r="5">
@@ -1551,7 +2001,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>29.05323542902901</v>
+        <v>31.89373538438543</v>
       </c>
     </row>
     <row r="6">
@@ -1561,136 +2011,226 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>29.91238277957146</v>
+        <v>33.05683304940691</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Training Total Number of Instances</t>
+          <t>Training Slope</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>175</v>
+        <v>1.281469479579516</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CV Correlation coefficient</t>
+          <t>Training Offset</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.6481357145715201</v>
+        <v>-145.0367251796205</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CV Mean absolute error</t>
+          <t>Training R²</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>64.5602670857143</v>
+        <v>0.890724578874364</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CV Root mean squared error</t>
+          <t>Training Total Number of Instances</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>78.37249943481655</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CV Relative absolute error</t>
+          <t>CV Correlation coefficient</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>77.52946281306575</v>
+        <v>0.6340983004477679</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CV Root relative squared error</t>
+          <t>CV Mean absolute error</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>76.25887161569855</v>
+        <v>64.18576105370857</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CV Total Number of Instances</t>
+          <t>CV Root mean squared error</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>175</v>
+        <v>79.69027806403592</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Validation Correlation coefficient</t>
+          <t>CV Relative absolute error</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.7391496613726907</v>
+        <v>77.07972409926663</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Validation Mean absolute error</t>
+          <t>CV Root relative squared error</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>41.76594853333334</v>
+        <v>77.54111107505295</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Validation Root mean squared error</t>
+          <t>CV Slope</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>52.76695096408437</v>
+        <v>1.098760765954987</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Validation Relative absolute error</t>
+          <t>CV Offset</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>65.80983774933166</v>
+        <v>-51.76325009283346</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Validation Root relative squared error</t>
+          <t>CV R²</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>68.30548679420436</v>
+        <v>0.39873760932463</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>CV Total Number of Instances</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Validation Correlation coefficient</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.7492464835117572</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Validation Mean absolute error</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>42.41097388794955</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Validation Root mean squared error</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>51.97893041055239</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Validation Relative absolute error</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>66.82619234972147</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Validation Root relative squared error</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>67.28541406820059</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Validation Slope</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1.032553112109504</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Validation Offset</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>-25.63169085405656</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Validation R²</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.5472673053670791</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>Validation Total Number of Instances</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B28" t="n">
         <v>75</v>
       </c>
     </row>
@@ -1705,7 +2245,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1732,7 +2272,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9779672599338202</v>
+        <v>0.9643521567971403</v>
       </c>
     </row>
     <row r="3">
@@ -1742,7 +2282,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.414288647736371</v>
+        <v>0.5004448208343442</v>
       </c>
     </row>
     <row r="4">
@@ -1752,7 +2292,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.7536886246305649</v>
+        <v>0.9562749331613076</v>
       </c>
     </row>
     <row r="5">
@@ -1762,7 +2302,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>16.77825339543587</v>
+        <v>20.26748756035243</v>
       </c>
     </row>
     <row r="6">
@@ -1772,136 +2312,226 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>23.43252451530416</v>
+        <v>29.73102562833143</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Training Total Number of Instances</t>
+          <t>Training Slope</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>175</v>
+        <v>1.163513968407607</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CV Correlation coefficient</t>
+          <t>Training Offset</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.8147380565663426</v>
+        <v>-2.505068097856638</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CV Mean absolute error</t>
+          <t>Training R²</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.097192913686986</v>
+        <v>0.91160661150875</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CV Root mean squared error</t>
+          <t>Training Total Number of Instances</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.87616558300909</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CV Relative absolute error</t>
+          <t>CV Correlation coefficient</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>44.4351560925011</v>
+        <v>0.8008628746855191</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CV Root relative squared error</t>
+          <t>CV Mean absolute error</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>58.33084722511222</v>
+        <v>1.105686558701478</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CV Total Number of Instances</t>
+          <t>CV Root mean squared error</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>175</v>
+        <v>1.950463780084701</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Validation Correlation coefficient</t>
+          <t>CV Relative absolute error</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.8904764239005015</v>
+        <v>44.779139759644</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Validation Mean absolute error</t>
+          <t>CV Root relative squared error</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.7784002501656637</v>
+        <v>60.64081219940189</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Validation Root mean squared error</t>
+          <t>CV Slope</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1.020029233735557</v>
+        <v>1.135322784402985</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Validation Relative absolute error</t>
+          <t>CV Offset</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>43.86958471955906</v>
+        <v>-2.07762136126839</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Validation Root relative squared error</t>
+          <t>CV R²</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>47.07059677007229</v>
+        <v>0.6322691895796873</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>CV Total Number of Instances</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Validation Correlation coefficient</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.8843898086409869</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Validation Mean absolute error</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.7570982105602236</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Validation Root mean squared error</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1.026593601465011</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Validation Relative absolute error</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>42.66903059464535</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Validation Root relative squared error</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>47.37351819254177</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Validation Slope</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.9225390409834219</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Validation Offset</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1.240889544093664</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Validation R²</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.7755749774060914</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>Validation Total Number of Instances</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B28" t="n">
         <v>75</v>
       </c>
     </row>
@@ -1916,7 +2546,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1943,7 +2573,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9570388994934571</v>
+        <v>0.9428518186918287</v>
       </c>
     </row>
     <row r="3">
@@ -1953,7 +2583,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.09446777142857139</v>
+        <v>0.115233616508888</v>
       </c>
     </row>
     <row r="4">
@@ -1963,7 +2593,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1880666890531882</v>
+        <v>0.2166579758056639</v>
       </c>
     </row>
     <row r="5">
@@ -1973,7 +2603,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>20.90715384676533</v>
+        <v>25.5029510301523</v>
       </c>
     </row>
     <row r="6">
@@ -1983,136 +2613,226 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>32.07020926551027</v>
+        <v>36.94575928416769</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Training Total Number of Instances</t>
+          <t>Training Slope</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>175</v>
+        <v>1.203590654479478</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CV Correlation coefficient</t>
+          <t>Training Offset</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.6509053820109231</v>
+        <v>-0.2326225102638753</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CV Mean absolute error</t>
+          <t>Training R²</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2599973714285714</v>
+        <v>0.8635010870916338</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CV Root mean squared error</t>
+          <t>Training Total Number of Instances</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.4466391184991685</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CV Relative absolute error</t>
+          <t>CV Correlation coefficient</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>57.54137058607157</v>
+        <v>0.658121720162785</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CV Root relative squared error</t>
+          <t>CV Mean absolute error</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>76.16346131547189</v>
+        <v>0.2594854819928088</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CV Total Number of Instances</t>
+          <t>CV Root mean squared error</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>175</v>
+        <v>0.4420470193132467</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Validation Correlation coefficient</t>
+          <t>CV Relative absolute error</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.7350230011562877</v>
+        <v>57.42808167257036</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Validation Mean absolute error</t>
+          <t>CV Root relative squared error</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.2157167999999999</v>
+        <v>75.38039025380799</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Validation Root mean squared error</t>
+          <t>CV Slope</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.3085260004083934</v>
+        <v>0.9566214532836544</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Validation Relative absolute error</t>
+          <t>CV Offset</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>60.66452620548425</v>
+        <v>0.03675242099834497</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Validation Root relative squared error</t>
+          <t>CV R²</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>70.53934520468439</v>
+        <v>0.4317796765183608</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>CV Total Number of Instances</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Validation Correlation coefficient</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.7673217788995015</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Validation Mean absolute error</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.2043389949494949</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Validation Root mean squared error</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.2879159719317281</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Validation Relative absolute error</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>57.46482570627764</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Validation Root relative squared error</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>65.82720453754625</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Validation Slope</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.8850721577634114</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Validation Offset</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.08347428370267762</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Validation R²</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.566677914277205</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>Validation Total Number of Instances</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B28" t="n">
         <v>75</v>
       </c>
     </row>
@@ -2127,7 +2847,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2154,7 +2874,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9663105194254217</v>
+        <v>0.9611210438139298</v>
       </c>
     </row>
     <row r="3">
@@ -2164,7 +2884,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.0577688000000001</v>
+        <v>0.06278857026921492</v>
       </c>
     </row>
     <row r="4">
@@ -2174,7 +2894,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.09398770053272172</v>
+        <v>0.1051473006590376</v>
       </c>
     </row>
     <row r="5">
@@ -2184,7 +2904,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>24.08134194679477</v>
+        <v>26.17386947631444</v>
       </c>
     </row>
     <row r="6">
@@ -2194,136 +2914,226 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>30.47387433296177</v>
+        <v>34.09218023818028</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Training Total Number of Instances</t>
+          <t>Training Slope</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>175</v>
+        <v>1.26239494238355</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CV Correlation coefficient</t>
+          <t>Training Offset</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.5569421037627067</v>
+        <v>-0.8651407465158059</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CV Mean absolute error</t>
+          <t>Training R²</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1520145142857143</v>
+        <v>0.8837723246607431</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CV Root mean squared error</t>
+          <t>Training Total Number of Instances</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.256916325415772</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CV Relative absolute error</t>
+          <t>CV Correlation coefficient</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>63.36834934065097</v>
+        <v>0.5716322082951938</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CV Root relative squared error</t>
+          <t>CV Mean absolute error</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>83.30064221627393</v>
+        <v>0.1526541444055944</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CV Total Number of Instances</t>
+          <t>CV Root mean squared error</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>175</v>
+        <v>0.2534060336270441</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Validation Correlation coefficient</t>
+          <t>CV Relative absolute error</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.4706613765154266</v>
+        <v>63.63498378063072</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Validation Mean absolute error</t>
+          <t>CV Root relative squared error</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.1774058666666668</v>
+        <v>82.16249126423016</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Validation Root mean squared error</t>
+          <t>CV Slope</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.2701399696058818</v>
+        <v>0.9619709255147016</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Validation Relative absolute error</t>
+          <t>CV Offset</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>75.28846893800281</v>
+        <v>0.1141270647214379</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Validation Root relative squared error</t>
+          <t>CV R²</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>102.5066380735386</v>
+        <v>0.3249325029255303</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>CV Total Number of Instances</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Validation Correlation coefficient</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.5741037342321906</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Validation Mean absolute error</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.1589244830895956</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Validation Root mean squared error</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.2253394942445595</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Validation Relative absolute error</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>67.44523861243501</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Validation Root relative squared error</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>85.50676160177653</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Validation Slope</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.7009159171771773</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Validation Offset</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.9893678458624304</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Validation R²</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.2688593720376955</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>Validation Total Number of Instances</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B28" t="n">
         <v>75</v>
       </c>
     </row>
@@ -2338,7 +3148,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2365,7 +3175,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9666961090100049</v>
+        <v>0.9573574846343409</v>
       </c>
     </row>
     <row r="3">
@@ -2375,7 +3185,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>22.78598000000001</v>
+        <v>26.95736439216655</v>
       </c>
     </row>
     <row r="4">
@@ -2385,7 +3195,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>29.45041399659692</v>
+        <v>33.81035295636499</v>
       </c>
     </row>
     <row r="5">
@@ -2395,7 +3205,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>27.36428142111235</v>
+        <v>32.37380641950525</v>
       </c>
     </row>
     <row r="6">
@@ -2405,136 +3215,226 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>28.65662277058594</v>
+        <v>32.89904619075557</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Training Total Number of Instances</t>
+          <t>Training Slope</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>175</v>
+        <v>1.196396361821014</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CV Correlation coefficient</t>
+          <t>Training Offset</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.676374774535864</v>
+        <v>-101.7812523191545</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CV Mean absolute error</t>
+          <t>Training R²</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>61.00318274285715</v>
+        <v>0.8917652759738531</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CV Root mean squared error</t>
+          <t>Training Total Number of Instances</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>75.82549623267161</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CV Relative absolute error</t>
+          <t>CV Correlation coefficient</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>73.26032324082995</v>
+        <v>0.6700017878499044</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CV Root relative squared error</t>
+          <t>CV Mean absolute error</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>73.78173502699286</v>
+        <v>61.91171394875978</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CV Total Number of Instances</t>
+          <t>CV Root mean squared error</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>175</v>
+        <v>76.37075994436351</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Validation Correlation coefficient</t>
+          <t>CV Relative absolute error</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.7176129869881022</v>
+        <v>74.35140221123991</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Validation Mean absolute error</t>
+          <t>CV Root relative squared error</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>46.35441466666666</v>
+        <v>74.31230198263056</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Validation Root mean squared error</t>
+          <t>CV Slope</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>56.63449561441841</v>
+        <v>0.9521939804199422</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Validation Relative absolute error</t>
+          <t>CV Offset</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>73.03165408995615</v>
+        <v>24.68540545317506</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Validation Root relative squared error</t>
+          <t>CV R²</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>73.30807771437706</v>
+        <v>0.4477681774042322</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>CV Total Number of Instances</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Validation Correlation coefficient</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.6983618569253621</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Validation Mean absolute error</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>46.64387526746633</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Validation Root mean squared error</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>57.21316697697413</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Validation Relative absolute error</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>73.48770097615434</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Validation Root relative squared error</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>74.05711387612084</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Validation Slope</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.8456170276670261</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Validation Offset</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>68.31491226482876</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Validation R²</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.451554388433927</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>Validation Total Number of Instances</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B28" t="n">
         <v>75</v>
       </c>
     </row>
@@ -2549,7 +3449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2576,7 +3476,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.974102633504475</v>
+        <v>0.9639624416044765</v>
       </c>
     </row>
     <row r="3">
@@ -2586,7 +3486,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.4828906197935105</v>
+        <v>0.5463716096920572</v>
       </c>
     </row>
     <row r="4">
@@ -2596,7 +3496,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8024677973593545</v>
+        <v>0.9345642316372005</v>
       </c>
     </row>
     <row r="5">
@@ -2606,7 +3506,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>19.54516145911544</v>
+        <v>22.11457603519922</v>
       </c>
     </row>
     <row r="6">
@@ -2616,136 +3516,226 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>24.94593172943042</v>
+        <v>29.05235025742611</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Training Total Number of Instances</t>
+          <t>Training Slope</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>175</v>
+        <v>1.137761466285982</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CV Correlation coefficient</t>
+          <t>Training Offset</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.7693139524868523</v>
+        <v>-2.120872564493546</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CV Mean absolute error</t>
+          <t>Training R²</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.259866436668793</v>
+        <v>0.9155960944519833</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CV Root mean squared error</t>
+          <t>Training Total Number of Instances</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2.055459023615205</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CV Relative absolute error</t>
+          <t>CV Correlation coefficient</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>50.99352091813591</v>
+        <v>0.7743070672141561</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CV Root relative squared error</t>
+          <t>CV Mean absolute error</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>63.89706932100718</v>
+        <v>1.249207947714331</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CV Total Number of Instances</t>
+          <t>CV Root mean squared error</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>175</v>
+        <v>2.035696379550787</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Validation Correlation coefficient</t>
+          <t>CV Relative absolute error</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.8213510216969492</v>
+        <v>50.56211496617471</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Validation Mean absolute error</t>
+          <t>CV Root relative squared error</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1.046325863511905</v>
+        <v>63.28271747879459</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Validation Root mean squared error</t>
+          <t>CV Slope</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1.411185922223095</v>
+        <v>1.00238734954422</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Validation Relative absolute error</t>
+          <t>CV Offset</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>58.93585710946873</v>
+        <v>-0.02283825790804705</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Validation Root relative squared error</t>
+          <t>CV R²</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>65.11869290733566</v>
+        <v>0.5995297668499066</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>CV Total Number of Instances</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Validation Correlation coefficient</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.8309406678099488</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Validation Mean absolute error</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.9710223285629246</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Validation Root mean squared error</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1.320209895054242</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Validation Relative absolute error</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>54.69427374585489</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Validation Root relative squared error</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>60.92063517316747</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Validation Slope</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.773482761420492</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Validation Offset</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>3.361770633659328</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Validation R²</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.6288676210097831</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>Validation Total Number of Instances</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B28" t="n">
         <v>75</v>
       </c>
     </row>
@@ -2760,7 +3750,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2787,7 +3777,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9774442164554856</v>
+        <v>0.9717768815692304</v>
       </c>
     </row>
     <row r="3">
@@ -2797,7 +3787,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.4507428571428574</v>
+        <v>0.50404968099361</v>
       </c>
     </row>
     <row r="4">
@@ -2807,7 +3797,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5750616563216756</v>
+        <v>0.6511482575232879</v>
       </c>
     </row>
     <row r="5">
@@ -2817,7 +3807,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>21.05609977089062</v>
+        <v>23.54628632334218</v>
       </c>
     </row>
     <row r="6">
@@ -2827,136 +3817,226 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>22.09422236403185</v>
+        <v>25.01751635762665</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Training Total Number of Instances</t>
+          <t>Training Slope</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>175</v>
+        <v>1.093744470708313</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CV Correlation coefficient</t>
+          <t>Training Offset</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.826514494367902</v>
+        <v>-1.306938509745914</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CV Mean absolute error</t>
+          <t>Training R²</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.166525714285714</v>
+        <v>0.9374123875295883</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CV Root mean squared error</t>
+          <t>Training Total Number of Instances</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.467383513994504</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CV Relative absolute error</t>
+          <t>CV Correlation coefficient</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>54.49333569256022</v>
+        <v>0.8291355412297043</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CV Root relative squared error</t>
+          <t>CV Mean absolute error</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>56.37777670464894</v>
+        <v>1.168229543690437</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CV Total Number of Instances</t>
+          <t>CV Root mean squared error</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>175</v>
+        <v>1.455109512162845</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Validation Correlation coefficient</t>
+          <t>CV Relative absolute error</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.8365664983494701</v>
+        <v>54.57292874959903</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Validation Mean absolute error</t>
+          <t>CV Root relative squared error</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9879733333333335</v>
+        <v>55.90620200864191</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Validation Root mean squared error</t>
+          <t>CV Slope</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1.301326769109127</v>
+        <v>0.9951987293088604</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Validation Relative absolute error</t>
+          <t>CV Offset</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>53.15189946057615</v>
+        <v>0.06606075580630666</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Validation Root relative squared error</t>
+          <t>CV R²</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>57.92550463404433</v>
+        <v>0.6874496576968925</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>CV Total Number of Instances</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Validation Correlation coefficient</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.8535499595782413</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Validation Mean absolute error</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.9523763077200577</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Validation Root mean squared error</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1.206964297040308</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Validation Relative absolute error</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>51.23681788635108</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Validation Root relative squared error</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>53.72518082387307</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Validation Slope</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.8770574448929697</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Validation Offset</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1.634789736498311</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Validation R²</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.711360494544214</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>Validation Total Number of Instances</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B28" t="n">
         <v>75</v>
       </c>
     </row>
@@ -2971,7 +4051,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2998,7 +4078,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9655988941612088</v>
+        <v>0.9409906107094673</v>
       </c>
     </row>
     <row r="3">
@@ -3008,7 +4088,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.09766868571428572</v>
+        <v>0.1116429777391259</v>
       </c>
     </row>
     <row r="4">
@@ -3018,7 +4098,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1627116566129</v>
+        <v>0.2073996702996538</v>
       </c>
     </row>
     <row r="5">
@@ -3028,7 +4108,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>23.11979783901139</v>
+        <v>26.42774453855787</v>
       </c>
     </row>
     <row r="6">
@@ -3038,136 +4118,226 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>29.09837160455102</v>
+        <v>37.09010652751368</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Training Total Number of Instances</t>
+          <t>Training Slope</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>175</v>
+        <v>1.18981238343393</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CV Correlation coefficient</t>
+          <t>Training Offset</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.5975209813550756</v>
+        <v>-0.2284282187486297</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CV Mean absolute error</t>
+          <t>Training R²</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2633150857142857</v>
+        <v>0.8624323997777688</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CV Root mean squared error</t>
+          <t>Training Total Number of Instances</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.4541557405195459</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CV Relative absolute error</t>
+          <t>CV Correlation coefficient</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>62.33104812616309</v>
+        <v>0.6088358905752017</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CV Root relative squared error</t>
+          <t>CV Mean absolute error</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>81.21847431876047</v>
+        <v>0.262410246280307</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CV Total Number of Instances</t>
+          <t>CV Root mean squared error</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>175</v>
+        <v>0.4474788278808566</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Validation Correlation coefficient</t>
+          <t>CV Relative absolute error</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.8325560944477886</v>
+        <v>62.11685762449554</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Validation Mean absolute error</t>
+          <t>CV Root relative squared error</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.1839365333333333</v>
+        <v>80.02441552066266</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Validation Root mean squared error</t>
+          <t>CV Slope</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.2853242500174145</v>
+        <v>0.8688365080706844</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Validation Relative absolute error</t>
+          <t>CV Offset</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>43.75307645855852</v>
+        <v>0.1227256733041502</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Validation Root relative squared error</t>
+          <t>CV R²</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>55.55539056637485</v>
+        <v>0.3596092920576325</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>CV Total Number of Instances</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Validation Correlation coefficient</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.8302973250784427</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Validation Mean absolute error</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.1862581212481962</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Validation Root mean squared error</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.2867971642243086</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Validation Relative absolute error</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>44.3053137531485</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Validation Root relative squared error</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>55.84218120555035</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Validation Slope</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1.024319533914383</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Validation Offset</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>-0.04180080269697317</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Validation R²</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.688165079820648</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>Validation Total Number of Instances</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B28" t="n">
         <v>75</v>
       </c>
     </row>
@@ -3182,7 +4352,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3209,7 +4379,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9660496546901577</v>
+        <v>0.9450738908012912</v>
       </c>
     </row>
     <row r="3">
@@ -3219,7 +4389,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.06160171428571437</v>
+        <v>0.0711362323559377</v>
       </c>
     </row>
     <row r="4">
@@ -3229,7 +4399,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.09410461404203305</v>
+        <v>0.1201777912706939</v>
       </c>
     </row>
     <row r="5">
@@ -3239,7 +4409,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>24.77414331649906</v>
+        <v>28.60860668922115</v>
       </c>
     </row>
     <row r="6">
@@ -3249,136 +4419,226 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>30.05200952040478</v>
+        <v>38.3783958329073</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Training Total Number of Instances</t>
+          <t>Training Slope</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>175</v>
+        <v>1.270128863423822</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CV Correlation coefficient</t>
+          <t>Training Offset</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.5448479792302328</v>
+        <v>-0.8947373212162333</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CV Mean absolute error</t>
+          <t>Training R²</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1654674448979593</v>
+        <v>0.8527098733292684</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CV Root mean squared error</t>
+          <t>Training Total Number of Instances</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.2658446710058855</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CV Relative absolute error</t>
+          <t>CV Correlation coefficient</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>66.54545643168242</v>
+        <v>0.5794309813066961</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CV Root relative squared error</t>
+          <t>CV Mean absolute error</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>84.89665108715374</v>
+        <v>0.1627999088373928</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CV Total Number of Instances</t>
+          <t>CV Root mean squared error</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>175</v>
+        <v>0.2555292333485883</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Validation Correlation coefficient</t>
+          <t>CV Relative absolute error</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.6809410567325063</v>
+        <v>65.47266289934839</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Validation Mean absolute error</t>
+          <t>CV Root relative squared error</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.1188869333333334</v>
+        <v>81.60244884383152</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Validation Root mean squared error</t>
+          <t>CV Slope</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.183969412559081</v>
+        <v>0.9651009877148174</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Validation Relative absolute error</t>
+          <t>CV Offset</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>56.15842352419538</v>
+        <v>0.1047564986299698</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Validation Root relative squared error</t>
+          <t>CV R²</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>74.51983882674787</v>
+        <v>0.334104034268986</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>CV Total Number of Instances</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Validation Correlation coefficient</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.7105794114725684</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Validation Mean absolute error</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.1191903751308877</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Validation Root mean squared error</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.1747408087078403</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Validation Relative absolute error</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>56.30175982284661</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Validation Root relative squared error</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>70.78164092730354</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Validation Slope</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.9658237302434293</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Validation Offset</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.09379614683818804</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Validation R²</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.4989959307638269</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>Validation Total Number of Instances</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B28" t="n">
         <v>75</v>
       </c>
     </row>
@@ -3393,7 +4653,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3420,7 +4680,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9713171939220724</v>
+        <v>0.9584403942637103</v>
       </c>
     </row>
     <row r="3">
@@ -3430,7 +4690,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>22.80388857142857</v>
+        <v>26.45745069185754</v>
       </c>
     </row>
     <row r="4">
@@ -3440,7 +4700,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>28.90412412750656</v>
+        <v>33.44193985474189</v>
       </c>
     </row>
     <row r="5">
@@ -3450,7 +4710,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>28.19579104315449</v>
+        <v>32.71322559332455</v>
       </c>
     </row>
     <row r="6">
@@ -3460,136 +4720,226 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>28.59250430938513</v>
+        <v>33.08139714570872</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Training Total Number of Instances</t>
+          <t>Training Slope</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>175</v>
+        <v>1.211523124116033</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CV Correlation coefficient</t>
+          <t>Training Offset</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.5994456471820345</v>
+        <v>-109.5655359358734</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CV Mean absolute error</t>
+          <t>Training R²</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>65.99048925714284</v>
+        <v>0.8905621162887895</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CV Root mean squared error</t>
+          <t>Training Total Number of Instances</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>81.61795856339307</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CV Relative absolute error</t>
+          <t>CV Correlation coefficient</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>81.59371767239644</v>
+        <v>0.6371471334997242</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CV Root relative squared error</t>
+          <t>CV Mean absolute error</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>80.73802276977524</v>
+        <v>62.90906117879737</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CV Total Number of Instances</t>
+          <t>CV Root mean squared error</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>175</v>
+        <v>78.05781605121979</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Validation Correlation coefficient</t>
+          <t>CV Relative absolute error</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.7798598283746856</v>
+        <v>77.78369632715992</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Validation Mean absolute error</t>
+          <t>CV Root relative squared error</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>45.31088106666666</v>
+        <v>77.21626270286256</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Validation Root mean squared error</t>
+          <t>CV Slope</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>52.65128148262625</v>
+        <v>0.9323897908173686</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Validation Relative absolute error</t>
+          <t>CV Offset</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>67.53824403786577</v>
+        <v>34.04865714850348</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Validation Root relative squared error</t>
+          <t>CV R²</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>64.31745730972872</v>
+        <v>0.4037648774202518</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>CV Total Number of Instances</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Validation Correlation coefficient</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.7651716027035574</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Validation Mean absolute error</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>47.40363733513526</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Validation Root mean squared error</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>54.31966176061668</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Validation Relative absolute error</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>70.65760698655016</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Validation Root relative squared error</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>66.35550793802068</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Validation Slope</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.9217011903464432</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Validation Offset</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>28.0358172358894</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Validation R²</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.5596946566287273</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>Validation Total Number of Instances</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B28" t="n">
         <v>75</v>
       </c>
     </row>

</xml_diff>